<commit_message>
change the calculation of materials
</commit_message>
<xml_diff>
--- a/Заказ №1 Этап №1.xlsx.xlsx
+++ b/Заказ №1 Этап №1.xlsx.xlsx
@@ -441,7 +441,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,7 +596,7 @@
         </is>
       </c>
       <c r="E2" s="1" t="n">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>4</v>
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="N2" s="1" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="O2" s="1" t="inlineStr">
         <is>
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="N3" s="2" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="O3" s="2" t="inlineStr"/>
       <c r="P3" s="2" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F4" s="2" t="n">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="N4" s="2" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="O4" s="2" t="inlineStr"/>
       <c r="P4" s="2" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
@@ -964,7 +964,7 @@
         </is>
       </c>
       <c r="N5" s="2" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="O5" s="2" t="inlineStr"/>
       <c r="P5" s="2" t="inlineStr"/>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F6" s="2" t="n">
@@ -1057,7 +1057,7 @@
         </is>
       </c>
       <c r="N6" s="2" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="O6" s="2" t="inlineStr"/>
       <c r="P6" s="2" t="inlineStr"/>
@@ -1111,24 +1111,24 @@
         </is>
       </c>
       <c r="E7" s="1" t="n">
-        <v>250</v>
+        <v>1250</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>4</v>
       </c>
       <c r="G7" s="1" t="inlineStr">
         <is>
-          <t>Стыковочный блок</t>
+          <t>Прямая секция</t>
         </is>
       </c>
       <c r="H7" s="1" t="inlineStr">
         <is>
-          <t>sb</t>
+          <t>pt3.0</t>
         </is>
       </c>
       <c r="I7" s="1" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3000</t>
         </is>
       </c>
       <c r="J7" s="1" t="inlineStr">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="N7" s="1" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="O7" s="1" t="inlineStr">
         <is>
@@ -1194,12 +1194,12 @@
           <t>Х</t>
         </is>
       </c>
-      <c r="W7" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="X7" s="1" t="inlineStr"/>
+      <c r="W7" s="1" t="inlineStr"/>
+      <c r="X7" s="1" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
       <c r="Y7" s="1" t="inlineStr"/>
     </row>
     <row r="8">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F8" s="2" t="n">
@@ -1231,16 +1231,16 @@
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>Стенка стыка</t>
+          <t>Крышка с выступом крашенная</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>СС</t>
+          <t>КВ-кр</t>
         </is>
       </c>
       <c r="I8" s="2" t="n">
-        <v>69</v>
+        <v>2763</v>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
@@ -1263,7 +1263,7 @@
         </is>
       </c>
       <c r="N8" s="2" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="O8" s="2" t="inlineStr"/>
       <c r="P8" s="2" t="inlineStr">
@@ -1287,7 +1287,11 @@
           <t>Х</t>
         </is>
       </c>
-      <c r="U8" s="2" t="inlineStr"/>
+      <c r="U8" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
       <c r="V8" s="2" t="inlineStr">
         <is>
           <t>Х</t>
@@ -1298,11 +1302,7 @@
           <t>Х</t>
         </is>
       </c>
-      <c r="X8" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
+      <c r="X8" s="2" t="inlineStr"/>
       <c r="Y8" s="2" t="inlineStr">
         <is>
           <t>Х</t>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="F9" s="2" t="n">
@@ -1338,16 +1338,16 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Пластина токопроводящая</t>
+          <t>Стенка крашенная</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>ТП</t>
+          <t>С-кр</t>
         </is>
       </c>
       <c r="I9" s="2" t="n">
-        <v>30</v>
+        <v>2762</v>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
@@ -1370,10 +1370,14 @@
         </is>
       </c>
       <c r="N9" s="2" t="n">
-        <v>240</v>
+        <v>2</v>
       </c>
       <c r="O9" s="2" t="inlineStr"/>
-      <c r="P9" s="2" t="inlineStr"/>
+      <c r="P9" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
       <c r="Q9" s="2" t="inlineStr">
         <is>
           <t>Х</t>
@@ -1384,13 +1388,21 @@
           <t>Х</t>
         </is>
       </c>
-      <c r="S9" s="2" t="inlineStr"/>
+      <c r="S9" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
       <c r="T9" s="2" t="inlineStr">
         <is>
           <t>Х</t>
         </is>
       </c>
-      <c r="U9" s="2" t="inlineStr"/>
+      <c r="U9" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
       <c r="V9" s="2" t="inlineStr">
         <is>
           <t>Х</t>
@@ -1429,7 +1441,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1250 (Алюм)</t>
         </is>
       </c>
       <c r="F10" s="2" t="n">
@@ -1437,21 +1449,19 @@
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>Втулка</t>
+          <t>Шина (СТП 05)</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>В</t>
+          <t>Ш1</t>
         </is>
       </c>
       <c r="I10" s="2" t="n">
-        <v>72</v>
-      </c>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>2959</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>2964</v>
       </c>
       <c r="K10" s="2" t="inlineStr">
         <is>
@@ -1469,21 +1479,21 @@
         </is>
       </c>
       <c r="N10" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O10" s="2" t="inlineStr"/>
-      <c r="P10" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="Q10" s="2" t="inlineStr"/>
-      <c r="R10" s="2" t="inlineStr"/>
-      <c r="S10" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
+      <c r="P10" s="2" t="inlineStr"/>
+      <c r="Q10" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="R10" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="S10" s="2" t="inlineStr"/>
       <c r="T10" s="2" t="inlineStr">
         <is>
           <t>Х</t>
@@ -1494,21 +1504,9 @@
           <t>Х</t>
         </is>
       </c>
-      <c r="V10" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="W10" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="X10" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
+      <c r="V10" s="2" t="inlineStr"/>
+      <c r="W10" s="2" t="inlineStr"/>
+      <c r="X10" s="2" t="inlineStr"/>
       <c r="Y10" s="2" t="inlineStr">
         <is>
           <t>Х</t>
@@ -1516,460 +1514,414 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>E3</t>
         </is>
       </c>
-      <c r="C11" s="1" t="inlineStr">
+      <c r="C11" s="2" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="D11" s="1" t="inlineStr">
+      <c r="D11" s="2" t="inlineStr">
         <is>
           <t>Al</t>
         </is>
       </c>
-      <c r="E11" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F11" s="1" t="n">
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>1250 (Алюм)</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="G11" s="1" t="inlineStr">
-        <is>
-          <t>Крышка стыка</t>
-        </is>
-      </c>
-      <c r="H11" s="1" t="inlineStr">
-        <is>
-          <t>КСБ</t>
-        </is>
-      </c>
-      <c r="I11" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J11" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K11" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L11" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M11" s="1" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N11" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="O11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="P11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="Q11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="R11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="S11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="T11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="U11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="V11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="W11" s="1" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="X11" s="1" t="inlineStr"/>
-      <c r="Y11" s="1" t="inlineStr">
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>Шина (СТП 06)</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr">
+        <is>
+          <t>Ш2</t>
+        </is>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>2959</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>2959.4</v>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L11" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M11" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="O11" s="2" t="inlineStr"/>
+      <c r="P11" s="2" t="inlineStr"/>
+      <c r="Q11" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="R11" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="S11" s="2" t="inlineStr"/>
+      <c r="T11" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="U11" s="2" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="V11" s="2" t="inlineStr"/>
+      <c r="W11" s="2" t="inlineStr"/>
+      <c r="X11" s="2" t="inlineStr"/>
+      <c r="Y11" s="2" t="inlineStr">
         <is>
           <t>Х</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="n">
+      <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="inlineStr">
+      <c r="B12" s="3" t="inlineStr">
         <is>
           <t>E3</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="D12" s="2" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>Al</t>
         </is>
       </c>
-      <c r="E12" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F12" s="2" t="n">
+      <c r="E12" s="3" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="F12" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>Демпфер</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="inlineStr">
-        <is>
-          <t>Д</t>
-        </is>
-      </c>
-      <c r="I12" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J12" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K12" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L12" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M12" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N12" s="2" t="n">
-        <v>120</v>
-      </c>
-      <c r="O12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="P12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="Q12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="R12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="S12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="T12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="U12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="V12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="W12" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="X12" s="2" t="inlineStr"/>
-      <c r="Y12" s="2" t="inlineStr">
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>Направляющая</t>
+        </is>
+      </c>
+      <c r="H12" s="3" t="inlineStr">
+        <is>
+          <t>Н</t>
+        </is>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>149</v>
+      </c>
+      <c r="J12" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K12" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O12" s="3" t="inlineStr"/>
+      <c r="P12" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="Q12" s="3" t="inlineStr"/>
+      <c r="R12" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="S12" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="T12" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="U12" s="3" t="inlineStr"/>
+      <c r="V12" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="W12" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="X12" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="Y12" s="3" t="inlineStr">
         <is>
           <t>Х</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="n">
+      <c r="A13" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="inlineStr">
+      <c r="B13" s="3" t="inlineStr">
         <is>
           <t>E3</t>
         </is>
       </c>
-      <c r="C13" s="2" t="inlineStr">
+      <c r="C13" s="3" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="D13" s="2" t="inlineStr">
+      <c r="D13" s="3" t="inlineStr">
         <is>
           <t>Al</t>
         </is>
       </c>
-      <c r="E13" s="2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="F13" s="2" t="n">
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G13" s="2" t="inlineStr">
-        <is>
-          <t>Изолятор крайний</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="inlineStr">
-        <is>
-          <t>ИК</t>
-        </is>
-      </c>
-      <c r="I13" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J13" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K13" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L13" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M13" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>60</v>
-      </c>
-      <c r="O13" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="P13" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="Q13" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="R13" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="S13" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="T13" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="U13" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="V13" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="W13" s="2" t="inlineStr"/>
-      <c r="X13" s="2" t="inlineStr"/>
-      <c r="Y13" s="2" t="inlineStr">
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>Сухарь</t>
+        </is>
+      </c>
+      <c r="H13" s="3" t="inlineStr">
+        <is>
+          <t>СУ</t>
+        </is>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="J13" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K13" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O13" s="3" t="inlineStr"/>
+      <c r="P13" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="Q13" s="3" t="inlineStr"/>
+      <c r="R13" s="3" t="inlineStr"/>
+      <c r="S13" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="T13" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="U13" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="V13" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="W13" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="X13" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="Y13" s="3" t="inlineStr">
         <is>
           <t>Х</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="n">
+      <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="inlineStr">
+      <c r="B14" s="3" t="inlineStr">
         <is>
           <t>E3</t>
         </is>
       </c>
-      <c r="C14" s="2" t="inlineStr">
+      <c r="C14" s="3" t="inlineStr">
         <is>
           <t>55</t>
         </is>
       </c>
-      <c r="D14" s="2" t="inlineStr">
+      <c r="D14" s="3" t="inlineStr">
         <is>
           <t>Al</t>
         </is>
       </c>
-      <c r="E14" s="2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="F14" s="2" t="n">
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>1250</t>
+        </is>
+      </c>
+      <c r="F14" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G14" s="2" t="inlineStr">
-        <is>
-          <t>Изолятор средний</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="inlineStr">
-        <is>
-          <t>ИС</t>
-        </is>
-      </c>
-      <c r="I14" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J14" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K14" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L14" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M14" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N14" s="2" t="n">
-        <v>90</v>
-      </c>
-      <c r="O14" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="P14" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="Q14" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="R14" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="S14" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="T14" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="U14" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="V14" s="2" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="W14" s="2" t="inlineStr"/>
-      <c r="X14" s="2" t="inlineStr"/>
-      <c r="Y14" s="2" t="inlineStr">
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>Направляющая</t>
+        </is>
+      </c>
+      <c r="H14" s="3" t="inlineStr">
+        <is>
+          <t>Н</t>
+        </is>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>179</v>
+      </c>
+      <c r="J14" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K14" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M14" s="3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N14" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O14" s="3" t="inlineStr"/>
+      <c r="P14" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="Q14" s="3" t="inlineStr"/>
+      <c r="R14" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="S14" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="T14" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="U14" s="3" t="inlineStr"/>
+      <c r="V14" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="W14" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="X14" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
+      <c r="Y14" s="3" t="inlineStr">
         <is>
           <t>Х</t>
         </is>
@@ -1996,7 +1948,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F15" s="3" t="n">
@@ -2004,16 +1956,16 @@
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>Направляющая</t>
+          <t>Сухарь</t>
         </is>
       </c>
       <c r="H15" s="3" t="inlineStr">
         <is>
-          <t>Н</t>
+          <t>СУ</t>
         </is>
       </c>
       <c r="I15" s="3" t="n">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="J15" s="3" t="inlineStr">
         <is>
@@ -2036,7 +1988,7 @@
         </is>
       </c>
       <c r="N15" s="3" t="n">
-        <v>120</v>
+        <v>4</v>
       </c>
       <c r="O15" s="3" t="inlineStr"/>
       <c r="P15" s="3" t="inlineStr">
@@ -2045,11 +1997,7 @@
         </is>
       </c>
       <c r="Q15" s="3" t="inlineStr"/>
-      <c r="R15" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
+      <c r="R15" s="3" t="inlineStr"/>
       <c r="S15" s="3" t="inlineStr">
         <is>
           <t>Х</t>
@@ -2060,7 +2008,11 @@
           <t>Х</t>
         </is>
       </c>
-      <c r="U15" s="3" t="inlineStr"/>
+      <c r="U15" s="3" t="inlineStr">
+        <is>
+          <t>Х</t>
+        </is>
+      </c>
       <c r="V15" s="3" t="inlineStr">
         <is>
           <t>Х</t>
@@ -2077,113 +2029,6 @@
         </is>
       </c>
       <c r="Y15" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
-      </c>
-      <c r="C16" s="3" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>Al</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>Сухарь</t>
-        </is>
-      </c>
-      <c r="H16" s="3" t="inlineStr">
-        <is>
-          <t>СУ</t>
-        </is>
-      </c>
-      <c r="I16" s="3" t="n">
-        <v>40</v>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K16" s="3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L16" s="3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M16" s="3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N16" s="3" t="n">
-        <v>120</v>
-      </c>
-      <c r="O16" s="3" t="inlineStr"/>
-      <c r="P16" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="Q16" s="3" t="inlineStr"/>
-      <c r="R16" s="3" t="inlineStr"/>
-      <c r="S16" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="T16" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="U16" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="V16" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="W16" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="X16" s="3" t="inlineStr">
-        <is>
-          <t>Х</t>
-        </is>
-      </c>
-      <c r="Y16" s="3" t="inlineStr">
         <is>
           <t>Х</t>
         </is>
@@ -2193,8 +2038,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 Ведомость Нач.смен&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 Ведомость Нач.смен&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -2209,7 +2054,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2312,7 +2157,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -2383,7 +2228,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -2454,7 +2299,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -2505,7 +2350,7 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -2525,7 +2370,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -2535,17 +2380,17 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>Изолятор крайний</t>
+          <t>Прямая секция</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>ИК</t>
+          <t>pt3.0</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3000</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
@@ -2569,14 +2414,14 @@
         </is>
       </c>
       <c r="N5" s="2">
-        <f>'Ведомость Нач.смен'!N13-'Ведомость Нач.смен'!W13</f>
+        <f>'Ведомость Нач.смен'!N7-'Ведомость Нач.смен'!W7</f>
         <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -2596,7 +2441,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1250 (Алюм)</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
@@ -2606,22 +2451,22 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Изолятор средний</t>
+          <t>Шина (СТП 05)</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>ИС</t>
+          <t>Ш1</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2959.0</t>
         </is>
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2964.0</t>
         </is>
       </c>
       <c r="K6" s="2" t="inlineStr">
@@ -2640,7 +2485,78 @@
         </is>
       </c>
       <c r="N6" s="2">
-        <f>'Ведомость Нач.смен'!N14-'Ведомость Нач.смен'!W14</f>
+        <f>'Ведомость Нач.смен'!N10-'Ведомость Нач.смен'!W10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>1250 (Алюм)</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>Шина (СТП 06)</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>Ш2</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>2959.0</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>2959.4</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M7" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N7" s="2">
+        <f>'Ведомость Нач.смен'!N11-'Ведомость Нач.смен'!W11</f>
         <v/>
       </c>
     </row>
@@ -2648,8 +2564,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 покраска&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 покраска&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -2664,7 +2580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2838,7 +2754,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -2909,7 +2825,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -2980,7 +2896,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -3031,7 +2947,7 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -3051,7 +2967,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
@@ -3061,17 +2977,17 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Стыковочный блок</t>
+          <t>Крышка с выступом крашенная</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>sb</t>
+          <t>КВ-кр</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2763.0</t>
         </is>
       </c>
       <c r="J6" s="2" t="inlineStr">
@@ -3095,7 +3011,7 @@
         </is>
       </c>
       <c r="N6" s="2">
-        <f>'Ведомость Нач.смен'!N7-'Ведомость Нач.смен'!X7</f>
+        <f>'Ведомость Нач.смен'!N8-'Ведомость Нач.смен'!X8</f>
         <v/>
       </c>
     </row>
@@ -3122,7 +3038,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -3132,17 +3048,17 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Пластина токопроводящая</t>
+          <t>Стенка крашенная</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>ТП</t>
+          <t>С-кр</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>2762.0</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
@@ -3173,7 +3089,7 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
@@ -3193,7 +3109,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1250 (Алюм)</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
@@ -3203,22 +3119,22 @@
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>Крышка стыка</t>
+          <t>Шина (СТП 05)</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>КСБ</t>
+          <t>Ш1</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2959.0</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2964.0</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -3237,14 +3153,14 @@
         </is>
       </c>
       <c r="N8" s="2">
-        <f>'Ведомость Нач.смен'!N11-'Ведомость Нач.смен'!X11</f>
+        <f>'Ведомость Нач.смен'!N10-'Ведомость Нач.смен'!X10</f>
         <v/>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -3264,7 +3180,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1250 (Алюм)</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
@@ -3274,22 +3190,22 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Демпфер</t>
+          <t>Шина (СТП 06)</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>Д</t>
+          <t>Ш2</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2959.0</t>
         </is>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2959.4</t>
         </is>
       </c>
       <c r="K9" s="2" t="inlineStr">
@@ -3308,149 +3224,7 @@
         </is>
       </c>
       <c r="N9" s="2">
-        <f>'Ведомость Нач.смен'!N12-'Ведомость Нач.смен'!X12</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>Al</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>Изолятор крайний</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>ИК</t>
-        </is>
-      </c>
-      <c r="I10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N10" s="2">
-        <f>'Ведомость Нач.смен'!N13-'Ведомость Нач.смен'!X13</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>Al</t>
-        </is>
-      </c>
-      <c r="E11" s="2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G11" s="2" t="inlineStr">
-        <is>
-          <t>Изолятор средний</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>ИС</t>
-        </is>
-      </c>
-      <c r="I11" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="J11" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K11" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L11" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M11" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N11" s="2">
-        <f>'Ведомость Нач.смен'!N14-'Ведомость Нач.смен'!X14</f>
+        <f>'Ведомость Нач.смен'!N11-'Ведомость Нач.смен'!X11</f>
         <v/>
       </c>
     </row>
@@ -3458,8 +3232,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 предсборка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 предсборка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -3577,7 +3351,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -3648,7 +3422,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -3658,17 +3432,17 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Стыковочный блок</t>
+          <t>Прямая секция</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>sb</t>
+          <t>pt3.0</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3000</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
@@ -3700,8 +3474,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 сборка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 сборка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -3716,7 +3490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3890,7 +3664,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -3961,7 +3735,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -4032,7 +3806,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -4103,7 +3877,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
@@ -4113,17 +3887,17 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Стенка стыка</t>
+          <t>Крышка с выступом крашенная</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>СС</t>
+          <t>КВ-кр</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>2763.0</t>
         </is>
       </c>
       <c r="J6" s="2" t="inlineStr">
@@ -4174,7 +3948,7 @@
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
@@ -4184,17 +3958,17 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Пластина токопроводящая</t>
+          <t>Стенка крашенная</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>ТП</t>
+          <t>С-кр</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>2762.0</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
@@ -4245,7 +4019,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1250 (Алюм)</t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
@@ -4255,22 +4029,22 @@
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>Втулка</t>
+          <t>Шина (СТП 05)</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
         <is>
-          <t>В</t>
+          <t>Ш1</t>
         </is>
       </c>
       <c r="I8" s="2" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>2959.0</t>
         </is>
       </c>
       <c r="J8" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2964.0</t>
         </is>
       </c>
       <c r="K8" s="2" t="inlineStr">
@@ -4296,7 +4070,7 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
@@ -4316,7 +4090,7 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>1250 (Алюм)</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
@@ -4326,22 +4100,22 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Направляющая</t>
+          <t>Шина (СТП 06)</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>Н</t>
+          <t>Ш2</t>
         </is>
       </c>
       <c r="I9" s="2" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>2959.0</t>
         </is>
       </c>
       <c r="J9" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2959.4</t>
         </is>
       </c>
       <c r="K9" s="2" t="inlineStr">
@@ -4360,14 +4134,14 @@
         </is>
       </c>
       <c r="N9" s="2">
-        <f>'Ведомость Нач.смен'!N15-'Ведомость Нач.смен'!O15</f>
+        <f>'Ведомость Нач.смен'!N11-'Ведомость Нач.смен'!O11</f>
         <v/>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
@@ -4387,7 +4161,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F10" s="2" t="inlineStr">
@@ -4397,41 +4171,254 @@
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
+          <t>Направляющая</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>Н</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>149</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L10" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M10" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N10" s="2">
+        <f>'Ведомость Нач.смен'!N12-'Ведомость Нач.смен'!O12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
           <t>Сухарь</t>
         </is>
       </c>
-      <c r="H10" s="2" t="inlineStr">
+      <c r="H11" s="2" t="inlineStr">
         <is>
           <t>СУ</t>
         </is>
       </c>
-      <c r="I10" s="2" t="inlineStr">
+      <c r="I11" s="2" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M10" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N10" s="2">
-        <f>'Ведомость Нач.смен'!N16-'Ведомость Нач.смен'!O16</f>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L11" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M11" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N11" s="2">
+        <f>'Ведомость Нач.смен'!N13-'Ведомость Нач.смен'!O13</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>1250</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>Направляющая</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="inlineStr">
+        <is>
+          <t>Н</t>
+        </is>
+      </c>
+      <c r="I12" s="2" t="inlineStr">
+        <is>
+          <t>179</t>
+        </is>
+      </c>
+      <c r="J12" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L12" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M12" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N12" s="2">
+        <f>'Ведомость Нач.смен'!N14-'Ведомость Нач.смен'!O14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G13" s="2" t="inlineStr">
+        <is>
+          <t>Сухарь</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="inlineStr">
+        <is>
+          <t>СУ</t>
+        </is>
+      </c>
+      <c r="I13" s="2" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="J13" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L13" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M13" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N13" s="2">
+        <f>'Ведомость Нач.смен'!N15-'Ведомость Нач.смен'!O15</f>
         <v/>
       </c>
     </row>
@@ -4439,8 +4426,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 пила&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 пила&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -4455,7 +4442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4558,7 +4545,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -4629,7 +4616,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -4680,7 +4667,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -4700,7 +4687,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1250 (Алюм)</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -4710,22 +4697,22 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>Пластина токопроводящая</t>
+          <t>Шина (СТП 05)</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>ТП</t>
+          <t>Ш1</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>2959.0</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2964.0</t>
         </is>
       </c>
       <c r="K4" s="2" t="inlineStr">
@@ -4744,7 +4731,78 @@
         </is>
       </c>
       <c r="N4" s="2">
-        <f>'Ведомость Нач.смен'!N9-'Ведомость Нач.смен'!P9</f>
+        <f>'Ведомость Нач.смен'!N10-'Ведомость Нач.смен'!P10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>1250 (Алюм)</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>Шина (СТП 06)</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>Ш2</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>2959.0</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>2959.4</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N5" s="2">
+        <f>'Ведомость Нач.смен'!N11-'Ведомость Нач.смен'!P11</f>
         <v/>
       </c>
     </row>
@@ -4752,8 +4810,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 гибка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 гибка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -4768,7 +4826,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4942,7 +5000,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -4952,17 +5010,17 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Стенка стыка</t>
+          <t>Крышка с выступом крашенная</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>СС</t>
+          <t>КВ-кр</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>2763.0</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
@@ -4993,7 +5051,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -5013,7 +5071,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1000</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -5023,17 +5081,17 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>Втулка</t>
+          <t>Направляющая</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>В</t>
+          <t>Н</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>149</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
@@ -5057,14 +5115,14 @@
         </is>
       </c>
       <c r="N4" s="2">
-        <f>'Ведомость Нач.смен'!N10-'Ведомость Нач.смен'!Q10</f>
+        <f>'Ведомость Нач.смен'!N12-'Ведомость Нач.смен'!Q12</f>
         <v/>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
@@ -5084,7 +5142,7 @@
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>250</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -5094,17 +5152,17 @@
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>Направляющая</t>
+          <t>Сухарь</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>Н</t>
+          <t>СУ</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>40</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
@@ -5128,14 +5186,14 @@
         </is>
       </c>
       <c r="N5" s="2">
-        <f>'Ведомость Нач.смен'!N15-'Ведомость Нач.смен'!Q15</f>
+        <f>'Ведомость Нач.смен'!N13-'Ведомость Нач.смен'!Q13</f>
         <v/>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
@@ -5155,7 +5213,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
@@ -5165,41 +5223,112 @@
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
+          <t>Направляющая</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>Н</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>179</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L6" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M6" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N6" s="2">
+        <f>'Ведомость Нач.смен'!N14-'Ведомость Нач.смен'!Q14</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
           <t>Сухарь</t>
         </is>
       </c>
-      <c r="H6" s="2" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>СУ</t>
         </is>
       </c>
-      <c r="I6" s="2" t="inlineStr">
+      <c r="I7" s="2" t="inlineStr">
         <is>
           <t>40</t>
         </is>
       </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L6" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N6" s="2">
-        <f>'Ведомость Нач.смен'!N16-'Ведомость Нач.смен'!Q16</f>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M7" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N7" s="2">
+        <f>'Ведомость Нач.смен'!N15-'Ведомость Нач.смен'!Q15</f>
         <v/>
       </c>
     </row>
@@ -5207,8 +5336,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 фрезер&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 фрезер&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -5306,7 +5435,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
@@ -5336,17 +5465,17 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Втулка</t>
+          <t>Сухарь</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>В</t>
+          <t>СУ</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>72</t>
+          <t>40</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
@@ -5370,14 +5499,14 @@
         </is>
       </c>
       <c r="N2" s="2">
-        <f>'Ведомость Нач.смен'!N10-'Ведомость Нач.смен'!R10</f>
+        <f>'Ведомость Нач.смен'!N13-'Ведомость Нач.смен'!R13</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -5441,7 +5570,7 @@
         </is>
       </c>
       <c r="N3" s="2">
-        <f>'Ведомость Нач.смен'!N16-'Ведомость Нач.смен'!R16</f>
+        <f>'Ведомость Нач.смен'!N15-'Ведомость Нач.смен'!R15</f>
         <v/>
       </c>
     </row>
@@ -5449,8 +5578,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 сверловка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 сверловка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -5465,7 +5594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5568,7 +5697,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
@@ -5639,7 +5768,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1000 (Алюм)</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -5690,7 +5819,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -5710,7 +5839,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1250 (Алюм)</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
@@ -5720,22 +5849,22 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>Пластина токопроводящая</t>
+          <t>Шина (СТП 05)</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>ТП</t>
+          <t>Ш1</t>
         </is>
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>2959.0</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>2964.0</t>
         </is>
       </c>
       <c r="K4" s="2" t="inlineStr">
@@ -5754,7 +5883,78 @@
         </is>
       </c>
       <c r="N4" s="2">
-        <f>'Ведомость Нач.смен'!N9-'Ведомость Нач.смен'!S9</f>
+        <f>'Ведомость Нач.смен'!N10-'Ведомость Нач.смен'!S10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>1250 (Алюм)</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>Шина (СТП 06)</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>Ш2</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>2959.0</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>2959.4</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N5" s="2">
+        <f>'Ведомость Нач.смен'!N11-'Ведомость Нач.смен'!S11</f>
         <v/>
       </c>
     </row>
@@ -5762,8 +5962,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 напыление&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 напыление&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -5862,8 +6062,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 сварка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 сварка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>
@@ -5873,319 +6073,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:N4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>№</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Серия</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ip</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Материал</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>In</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Кол. пров.</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Наименование</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Обозначение</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Разм.L</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Разм.L1</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Разм.A</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Разм.B</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Разм.C</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Кол.</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Al</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>Стенка стыка</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>СС</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M2" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N2" s="2">
-        <f>'Ведомость Нач.смен'!N8-'Ведомость Нач.смен'!U8</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Al</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>250 (Алюм)</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>Пластина токопроводящая</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>ТП</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L3" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M3" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N3" s="2">
-        <f>'Ведомость Нач.смен'!N9-'Ведомость Нач.смен'!U9</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>Al</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>Направляющая</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>Н</t>
-        </is>
-      </c>
-      <c r="I4" s="2" t="inlineStr">
-        <is>
-          <t>69</t>
-        </is>
-      </c>
-      <c r="J4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="L4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="M4" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="N4" s="2">
-        <f>'Ведомость Нач.смен'!N15-'Ведомость Нач.смен'!U15</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToHeight="0"/>
-  <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 зачистка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6274,52 +6161,52 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>E3</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>55</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>Al</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>250 (Алюм)</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Шина (СТП 05)</t>
+          <t>Направляющая</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>Ш1</t>
+          <t>Н</t>
         </is>
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>2959.0</t>
+          <t>149</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>2964.0</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K2" s="2" t="inlineStr">
@@ -6338,14 +6225,14 @@
         </is>
       </c>
       <c r="N2" s="2">
-        <f>'Ведомость Нач.смен'!N5-'Ведомость Нач.смен'!V5</f>
+        <f>'Ведомость Нач.смен'!N12-'Ведомость Нач.смен'!U12</f>
         <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
@@ -6365,7 +6252,7 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>250 (Алюм)</t>
+          <t>1250</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
@@ -6375,22 +6262,22 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Шина (СТП 06)</t>
+          <t>Направляющая</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>Ш2</t>
+          <t>Н</t>
         </is>
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>2959.0</t>
+          <t>179</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>2959.4</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K3" s="2" t="inlineStr">
@@ -6409,7 +6296,7 @@
         </is>
       </c>
       <c r="N3" s="2">
-        <f>'Ведомость Нач.смен'!N6-'Ведомость Нач.смен'!V6</f>
+        <f>'Ведомость Нач.смен'!N14-'Ведомость Нач.смен'!U14</f>
         <v/>
       </c>
     </row>
@@ -6417,8 +6304,392 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 шлифовка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_09 09 2021</oddHeader>
-    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_LAPTOP-MKGT243D</oddFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 зачистка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>№</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Серия</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Материал</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Кол. пров.</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Наименование</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Обозначение</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Разм.L</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Разм.L1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Разм.A</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Разм.B</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Разм.C</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Кол.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>1000 (Алюм)</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>Шина (СТП 05)</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>Ш1</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>2959.0</t>
+        </is>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>2964.0</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L2" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M2" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N2" s="2">
+        <f>'Ведомость Нач.смен'!N5-'Ведомость Нач.смен'!V5</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>1000 (Алюм)</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>Шина (СТП 06)</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>Ш2</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>2959.0</t>
+        </is>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>2959.4</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L3" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M3" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N3" s="2">
+        <f>'Ведомость Нач.смен'!N6-'Ведомость Нач.смен'!V6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>1250 (Алюм)</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>Шина (СТП 05)</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>Ш1</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>2959.0</t>
+        </is>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>2964.0</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M4" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N4" s="2">
+        <f>'Ведомость Нач.смен'!N10-'Ведомость Нач.смен'!V10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Al</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>1250 (Алюм)</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>Шина (СТП 06)</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>Ш2</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>2959.0</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>2959.4</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M5" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N5" s="2">
+        <f>'Ведомость Нач.смен'!N11-'Ведомость Нач.смен'!V11</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup fitToHeight="0"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1_x000a_Этап № 1&amp;C&amp;"Century Gothic"&amp;20 шлифовка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddFooter>&amp;L&amp;"Century Gothic"&amp;14 Время начала:____:_____x000a_Время завершения:____:____&amp;C&amp;"Century Gothic"&amp;14 ФИО исполнителя:____________&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>

</xml_diff>